<commit_message>
feat: added a mailing service that will deliver the generated excel to the user
</commit_message>
<xml_diff>
--- a/CustomersData.xlsx
+++ b/CustomersData.xlsx
@@ -4,10 +4,9 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Customers-1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -358,17 +357,6 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>

</xml_diff>